<commit_message>
Ajout de fonctions de manipulation des bases de données
</commit_message>
<xml_diff>
--- a/BDD_geometrie.xlsx
+++ b/BDD_geometrie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amark\PycharmProjects\PipeHelper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C7087F-759B-4A52-8173-87362F966EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A49881-150F-40D2-848F-509FFB3B6B7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="570" yWindow="1510" windowWidth="14400" windowHeight="8170" xr2:uid="{5F94B6D9-F312-4043-B946-45F3E89BC6EF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{5F94B6D9-F312-4043-B946-45F3E89BC6EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>coude</t>
   </si>
   <si>
-    <t>té</t>
-  </si>
-  <si>
     <t>angle</t>
   </si>
   <si>
@@ -63,13 +60,16 @@
     <t>agrandissement</t>
   </si>
   <si>
-    <t>rétrécissement</t>
-  </si>
-  <si>
-    <t>rapport diametre sortie entrée</t>
-  </si>
-  <si>
-    <t>rétrécissement brusque</t>
+    <t>rapport diametre sortie entree</t>
+  </si>
+  <si>
+    <t>te</t>
+  </si>
+  <si>
+    <t>retrecissement brusque</t>
+  </si>
+  <si>
+    <t>retrecissement</t>
   </si>
 </sst>
 </file>
@@ -423,11 +423,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EACA097E-C55E-4919-8BB8-75FA6CDFBF75}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" workbookViewId="0">
+      <selection activeCell="A7" sqref="A1:E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="26.6328125" customWidth="1"/>
+    <col min="4" max="4" width="25.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -437,10 +441,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -503,7 +507,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>15</v>
@@ -514,7 +518,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>30</v>
@@ -525,7 +529,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>45</v>
@@ -536,7 +540,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>60</v>
@@ -547,7 +551,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C11">
         <v>90</v>
@@ -558,7 +562,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12">
         <v>0.5</v>
@@ -569,7 +573,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13">
         <v>0.75</v>
@@ -580,7 +584,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -591,7 +595,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15">
         <v>1.5</v>
@@ -602,7 +606,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -613,7 +617,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17">
         <v>15</v>
@@ -624,7 +628,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18">
         <v>30</v>
@@ -635,7 +639,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19">
         <v>45</v>
@@ -646,7 +650,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20">
         <v>60</v>
@@ -657,7 +661,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21">
         <v>90</v>
@@ -668,7 +672,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C22">
         <v>5</v>
@@ -679,7 +683,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C23">
         <v>10</v>
@@ -690,7 +694,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C24">
         <v>15</v>
@@ -701,7 +705,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C25">
         <v>30</v>
@@ -712,7 +716,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C26">
         <v>45</v>
@@ -723,7 +727,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C27">
         <v>90</v>
@@ -734,7 +738,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D28">
         <v>0.1</v>
@@ -745,7 +749,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D29">
         <v>0.2</v>
@@ -756,7 +760,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D30">
         <v>0.4</v>
@@ -767,7 +771,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D31">
         <v>0.6</v>
@@ -778,7 +782,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D32">
         <v>0.8</v>
@@ -789,7 +793,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -800,7 +804,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C34">
         <v>15</v>
@@ -811,7 +815,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C35">
         <v>30</v>
@@ -822,7 +826,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C36">
         <v>45</v>
@@ -833,7 +837,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C37">
         <v>60</v>
@@ -844,7 +848,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C38">
         <v>90</v>

</xml_diff>

<commit_message>
Les fonctions de calculs et de tracage sont implémentées dans la Classe canalisation
Ajout de fonction dans main

Corrections mineures dans les autres fichiers

Problème de calcul de pression et vitesse
</commit_message>
<xml_diff>
--- a/BDD_geometrie.xlsx
+++ b/BDD_geometrie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amark\PycharmProjects\PipeHelper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A49881-150F-40D2-848F-509FFB3B6B7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABDB0978-9862-4C21-BD7E-407E425D7740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{5F94B6D9-F312-4043-B946-45F3E89BC6EF}"/>
+    <workbookView xWindow="7940" yWindow="1520" windowWidth="14400" windowHeight="8170" xr2:uid="{5F94B6D9-F312-4043-B946-45F3E89BC6EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="12">
   <si>
     <t>nom</t>
   </si>
@@ -421,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EACA097E-C55E-4919-8BB8-75FA6CDFBF75}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" workbookViewId="0">
-      <selection activeCell="A7" sqref="A1:E38"/>
+    <sheetView tabSelected="1" zoomScale="120" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -507,13 +507,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7">
-        <v>15</v>
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
       </c>
       <c r="E7">
-        <v>0.1</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -521,10 +521,10 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E8">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -532,10 +532,10 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="E9">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -543,10 +543,10 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -554,21 +554,21 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E11">
-        <v>1.4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12">
-        <v>0.5</v>
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>90</v>
       </c>
       <c r="E12">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -576,10 +576,10 @@
         <v>5</v>
       </c>
       <c r="B13">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="E13">
-        <v>0.8</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -587,10 +587,10 @@
         <v>5</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E14">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -598,10 +598,10 @@
         <v>5</v>
       </c>
       <c r="B15">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -609,21 +609,21 @@
         <v>5</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="E16">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17">
-        <v>15</v>
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
       </c>
       <c r="E17">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -631,10 +631,10 @@
         <v>6</v>
       </c>
       <c r="C18">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E18">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -642,10 +642,10 @@
         <v>6</v>
       </c>
       <c r="C19">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="E19">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -653,10 +653,10 @@
         <v>6</v>
       </c>
       <c r="C20">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="E20">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -664,21 +664,21 @@
         <v>6</v>
       </c>
       <c r="C21">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E21">
-        <v>1.3</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22">
-        <v>5</v>
+        <v>90</v>
       </c>
       <c r="E22">
-        <v>0.15</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -686,10 +686,10 @@
         <v>7</v>
       </c>
       <c r="C23">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E23">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -697,10 +697,10 @@
         <v>7</v>
       </c>
       <c r="C24">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E24">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -708,10 +708,10 @@
         <v>7</v>
       </c>
       <c r="C25">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E25">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -719,10 +719,10 @@
         <v>7</v>
       </c>
       <c r="C26">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="E26">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -730,21 +730,21 @@
         <v>7</v>
       </c>
       <c r="C27">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28">
-        <v>0.1</v>
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <v>90</v>
       </c>
       <c r="E28">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -752,10 +752,10 @@
         <v>10</v>
       </c>
       <c r="D29">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E29">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -763,10 +763,10 @@
         <v>10</v>
       </c>
       <c r="D30">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="E30">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -774,10 +774,10 @@
         <v>10</v>
       </c>
       <c r="D31">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="E31">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -785,21 +785,21 @@
         <v>10</v>
       </c>
       <c r="D32">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="E32">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="D33">
+        <v>0.8</v>
       </c>
       <c r="E33">
-        <v>0.9</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -807,10 +807,10 @@
         <v>11</v>
       </c>
       <c r="C34">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E34">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
@@ -818,10 +818,10 @@
         <v>11</v>
       </c>
       <c r="C35">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E35">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
@@ -829,7 +829,7 @@
         <v>11</v>
       </c>
       <c r="C36">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="E36">
         <v>0.3</v>
@@ -840,10 +840,10 @@
         <v>11</v>
       </c>
       <c r="C37">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="E37">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
@@ -851,9 +851,20 @@
         <v>11</v>
       </c>
       <c r="C38">
+        <v>60</v>
+      </c>
+      <c r="E38">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39">
         <v>90</v>
       </c>
-      <c r="E38">
+      <c r="E39">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>